<commit_message>
WRI LCFS and pumped hydro edits
</commit_message>
<xml_diff>
--- a/InputData/trans/BLP/BAU LCFS Perc.xlsx
+++ b/InputData/trans/BLP/BAU LCFS Perc.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\BLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAFB86EE-DC6A-4922-B6D3-09C903B16909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F58671C7-6C5F-4B29-BB58-3DCED3539B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="India Data" sheetId="6" r:id="rId2"/>
     <sheet name="BLP" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>BLP BAU LCFS Percentage</t>
   </si>
@@ -42,22 +41,85 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>India National Biofuel blending requirement</t>
+  </si>
+  <si>
+    <t>Current Progress on India's Ethanol Blending Program</t>
+  </si>
+  <si>
+    <t>Ministry of Petroleum and Natural Gas/ Press Information Bureau</t>
+  </si>
+  <si>
+    <t>NITI Aayog / Ministry of Petroleum and Natural Gas</t>
+  </si>
+  <si>
+    <t>National Policy on Biofuel</t>
+  </si>
+  <si>
+    <t>Roadmap for Ethanol Blending in India 2020-25</t>
+  </si>
+  <si>
+    <t>https://pib.gov.in/PressReleasePage.aspx?PRID=1575404</t>
+  </si>
+  <si>
+    <t>https://www.niti.gov.in/sites/default/files/2021-06/EthanolBlendingInIndia_compressed.pdf</t>
+  </si>
+  <si>
+    <t>Table 4.2, Pg. 25</t>
+  </si>
+  <si>
+    <t>Advancement of Ethanol blending target</t>
+  </si>
+  <si>
     <t>LCFS Achieved Before Fuel Shifts</t>
   </si>
   <si>
+    <t>Press Information Bureau, Govt. of India</t>
+  </si>
+  <si>
     <t>Data from Vensim variable for BAU scenario</t>
   </si>
   <si>
     <t>Variable name: "Achieved LCFS Percentage before Fuel Shifts"</t>
   </si>
   <si>
+    <t>https://pib.gov.in/PressReleseDetailm.aspx?PRID=1724642</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Trend-based achievement of India's ethanol blending target for petroleum is assumed for the BAU in the BPoEFUbVT variable, </t>
-  </si>
-  <si>
-    <t>The BAU LCFS percentage is set to the BAU Vensim variable "Achieved LCFS Percentage before Fuel Shifts" which accounts for BAU electricity and biofuel blending in transport.</t>
+    <t xml:space="preserve">MoPNG has announced the National Policy on Biofuels in 2018 with a target of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20% blending of ethanol in petrol and 5% blending of bio-diesel in diesel by 2030. </t>
+  </si>
+  <si>
+    <t>In 2021, the target for petrol was advanced to 2025 from 2030.</t>
+  </si>
+  <si>
+    <t>Due to feedstock supply procurement and land availability constraints, we</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjust this target to a more realistic level by extrapolating </t>
+  </si>
+  <si>
+    <t>the historical trend in target progress between 2014-2021 until 2025.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> We estimate the carbon intensity of the biofuel </t>
+  </si>
+  <si>
+    <t>per litre, relative to conventional petrol (using values from model input file fuels/PEI), to estimate the LCFS percentage.</t>
+  </si>
+  <si>
+    <t>Beyond 2025, we hold the values constant due to lack of credible projections</t>
+  </si>
+  <si>
+    <t>and long-term uncertaintly associated with bio-ethanol feedstock availability.</t>
+  </si>
+  <si>
+    <t>We do not consider the target for diesel as its blending staus as of 2021 is at less than 0.1%</t>
   </si>
   <si>
     <t xml:space="preserve">Since the model includes electricity as a carbon-free source in the LCFS policy, </t>
@@ -66,16 +128,52 @@
     <t xml:space="preserve">the LCFS policy setting should specify an LCFS percentage for biofuels in addition to </t>
   </si>
   <si>
-    <t xml:space="preserve">what is already achieved through BAU electricity-use in the transport sector, and the BAU blending rates already assumed to be achieved in the BPoEFUbVT variable, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">for this policy to take effect for biofuel blending mandates. </t>
-  </si>
-  <si>
-    <t>LCFS achieved before fuel shifts (Vensim)</t>
+    <t xml:space="preserve">what is already achieved through electricity-use in the transport sector for this policy to take effect for biofuel blending mandates. </t>
+  </si>
+  <si>
+    <t>Ethanol supply and Blending status since 2012-'13</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Blending %</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>CO2 emissions intensity (from file fuels/PEI)</t>
+  </si>
+  <si>
+    <t>Petroleum gasoline</t>
+  </si>
+  <si>
+    <t>g/BTU</t>
+  </si>
+  <si>
+    <t>Biofuel gasoline</t>
+  </si>
+  <si>
+    <t>|&lt;-- Historic progress</t>
+  </si>
+  <si>
+    <t>Carbon intensity ratio</t>
+  </si>
+  <si>
+    <t>|&lt;-- Trend based (2017-21) projections</t>
+  </si>
+  <si>
+    <t>LCFS achieved from biofuel gasoline shift</t>
+  </si>
+  <si>
+    <t>India LCFS %</t>
   </si>
   <si>
     <t>BAU LCFS Perc (dimensionless)</t>
+  </si>
+  <si>
+    <t>Achieved LCFS Percentage before Fuel Shifts</t>
   </si>
 </sst>
 </file>
@@ -155,7 +253,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,11 +268,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="53"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -219,6 +323,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="hair">
         <color indexed="64"/>
       </left>
@@ -255,25 +385,49 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="6" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Accent6 2" xfId="11" xr:uid="{083580D2-BB25-4950-82FB-4BC359D4A0E5}"/>
@@ -625,312 +779,894 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>2021</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{FB89C71C-543B-4451-B50F-90BB3D3CC750}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{DB2C66A2-500E-4EC9-85DD-D3844ACC5F91}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{DCCA8351-BB79-43B5-BBBE-AEF82B49DE3B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AI21"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection sqref="A1:XFD17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B1" s="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K3" s="13">
+        <v>2013</v>
+      </c>
+      <c r="L3" s="17">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="13">
+        <f>K3+1</f>
+        <v>2014</v>
+      </c>
+      <c r="L4" s="17">
+        <v>1.5300000000000001E-2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="14">
+        <v>7.3115370610735544E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="13">
+        <f t="shared" ref="K5:K6" si="0">K4+1</f>
+        <v>2015</v>
+      </c>
+      <c r="L5" s="17">
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4.2344979857895045E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="L6" s="17">
+        <v>3.5099999999999999E-2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K7" s="13">
+        <f>K6+1</f>
         <v>2017</v>
       </c>
-      <c r="C1" s="1">
+      <c r="L7" s="17">
+        <v>2.07E-2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <f>B6/B5</f>
+        <v>0.57915291277587433</v>
+      </c>
+      <c r="K8" s="13">
+        <f>K7+1</f>
         <v>2018</v>
       </c>
-      <c r="D1" s="1">
+      <c r="L8" s="17">
+        <v>4.2199999999999994E-2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="13">
+        <f>K8+1</f>
         <v>2019</v>
       </c>
-      <c r="E1" s="1">
+      <c r="L9" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="13">
+        <f t="shared" ref="K10:K15" si="1">K9+1</f>
         <v>2020</v>
       </c>
-      <c r="F1" s="1">
+      <c r="L10" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="M10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="13">
+        <f t="shared" si="1"/>
         <v>2021</v>
       </c>
-      <c r="G1" s="1">
+      <c r="L11" s="17">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="13">
+        <f t="shared" si="1"/>
         <v>2022</v>
       </c>
-      <c r="H1" s="1">
+      <c r="L12" s="18">
+        <f>TREND($L$7:$L$11,$K$7:$K$11,K12)</f>
+        <v>9.0499999999998693E-2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K13" s="13">
+        <f t="shared" si="1"/>
         <v>2023</v>
       </c>
-      <c r="I1" s="1">
+      <c r="L13" s="18">
+        <f t="shared" ref="L13:L15" si="2">TREND($L$7:$L$11,$K$7:$K$11,K13)</f>
+        <v>0.10413999999999746</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K14" s="13">
+        <f t="shared" si="1"/>
         <v>2024</v>
       </c>
-      <c r="J1" s="1">
+      <c r="L14" s="18">
+        <f t="shared" si="2"/>
+        <v>0.11777999999999977</v>
+      </c>
+      <c r="M14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" s="8">
+        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L15" s="18">
+        <f t="shared" si="2"/>
+        <v>0.13141999999999854</v>
+      </c>
+      <c r="M15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2024</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2025</v>
+      </c>
+      <c r="K18" s="1">
         <v>2026</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L18" s="1">
         <v>2027</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M18" s="1">
         <v>2028</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N18" s="1">
         <v>2029</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O18" s="1">
         <v>2030</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P18" s="1">
         <v>2031</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q18" s="1">
         <v>2032</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R18" s="1">
         <v>2033</v>
       </c>
-      <c r="S1" s="1">
+      <c r="S18" s="1">
         <v>2034</v>
       </c>
-      <c r="T1" s="1">
+      <c r="T18" s="1">
         <v>2035</v>
       </c>
-      <c r="U1" s="1">
+      <c r="U18" s="1">
         <v>2036</v>
       </c>
-      <c r="V1" s="1">
+      <c r="V18" s="1">
         <v>2037</v>
       </c>
-      <c r="W1" s="1">
+      <c r="W18" s="1">
         <v>2038</v>
       </c>
-      <c r="X1" s="1">
+      <c r="X18" s="1">
         <v>2039</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Y18" s="1">
         <v>2040</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Z18" s="1">
         <v>2041</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AA18" s="1">
         <v>2042</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AB18" s="1">
         <v>2043</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AC18" s="1">
         <v>2044</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AD18" s="1">
         <v>2045</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AE18" s="1">
         <v>2046</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AF18" s="1">
         <v>2047</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="AG18" s="1">
         <v>2048</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="AH18" s="1">
         <v>2049</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AI18" s="1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3">
-        <f>D2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="C2" s="3">
-        <f>D2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="D2" s="8">
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="E2" s="8">
-        <v>4.6217899999999999E-2</v>
-      </c>
-      <c r="F2" s="8">
-        <v>4.7382899999999999E-2</v>
-      </c>
-      <c r="G2" s="8">
-        <v>4.8742599999999997E-2</v>
-      </c>
-      <c r="H2" s="8">
-        <v>5.0532800000000003E-2</v>
-      </c>
-      <c r="I2" s="8">
-        <v>5.2832999999999998E-2</v>
-      </c>
-      <c r="J2" s="8">
-        <v>5.5727800000000001E-2</v>
-      </c>
-      <c r="K2" s="8">
-        <v>5.9197E-2</v>
-      </c>
-      <c r="L2" s="8">
-        <v>6.3418799999999997E-2</v>
-      </c>
-      <c r="M2" s="8">
-        <v>6.8455600000000005E-2</v>
-      </c>
-      <c r="N2" s="8">
-        <v>7.4057899999999996E-2</v>
-      </c>
-      <c r="O2" s="8">
-        <v>8.0028500000000002E-2</v>
-      </c>
-      <c r="P2" s="8">
-        <v>8.6307599999999998E-2</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>9.3254299999999998E-2</v>
-      </c>
-      <c r="R2" s="8">
-        <v>0.100676</v>
-      </c>
-      <c r="S2" s="8">
-        <v>0.10834299999999999</v>
-      </c>
-      <c r="T2" s="8">
-        <v>0.116036</v>
-      </c>
-      <c r="U2" s="8">
-        <v>0.123373</v>
-      </c>
-      <c r="V2" s="8">
-        <v>0.130523</v>
-      </c>
-      <c r="W2" s="8">
-        <v>0.137318</v>
-      </c>
-      <c r="X2" s="8">
-        <v>0.14362</v>
-      </c>
-      <c r="Y2" s="8">
-        <v>0.14927699999999999</v>
-      </c>
-      <c r="Z2" s="8">
-        <v>0.154227</v>
-      </c>
-      <c r="AA2" s="8">
-        <v>0.15858800000000001</v>
-      </c>
-      <c r="AB2" s="8">
-        <v>0.16231100000000001</v>
-      </c>
-      <c r="AC2" s="8">
-        <v>0.16545099999999999</v>
-      </c>
-      <c r="AD2" s="8">
-        <v>0.168075</v>
-      </c>
-      <c r="AE2" s="8">
-        <v>0.170241</v>
-      </c>
-      <c r="AF2" s="8">
-        <v>0.17203599999999999</v>
-      </c>
-      <c r="AG2" s="8">
-        <v>0.17349800000000001</v>
-      </c>
-      <c r="AH2" s="8">
-        <v>0.17466400000000001</v>
-      </c>
-      <c r="AI2" s="8">
-        <v>0.17560700000000001</v>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="14">
+        <f>D19</f>
+        <v>4.2300400000000002E-2</v>
+      </c>
+      <c r="C19" s="14">
+        <f>D19</f>
+        <v>4.2300400000000002E-2</v>
+      </c>
+      <c r="D19" s="16">
+        <v>4.2300400000000002E-2</v>
+      </c>
+      <c r="E19" s="16">
+        <v>4.28698E-2</v>
+      </c>
+      <c r="F19" s="16">
+        <v>4.3744499999999999E-2</v>
+      </c>
+      <c r="G19" s="16">
+        <v>4.4815500000000001E-2</v>
+      </c>
+      <c r="H19" s="16">
+        <v>4.6311699999999997E-2</v>
+      </c>
+      <c r="I19" s="16">
+        <v>4.8324499999999999E-2</v>
+      </c>
+      <c r="J19" s="16">
+        <v>5.0942000000000001E-2</v>
+      </c>
+      <c r="K19" s="16">
+        <v>5.4200999999999999E-2</v>
+      </c>
+      <c r="L19" s="16">
+        <v>5.8218300000000001E-2</v>
+      </c>
+      <c r="M19" s="16">
+        <v>6.3068200000000005E-2</v>
+      </c>
+      <c r="N19" s="16">
+        <v>6.84998E-2</v>
+      </c>
+      <c r="O19" s="16">
+        <v>7.4335300000000007E-2</v>
+      </c>
+      <c r="P19" s="16">
+        <v>8.0818200000000007E-2</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>8.7976299999999993E-2</v>
+      </c>
+      <c r="R19" s="16">
+        <v>9.5600599999999994E-2</v>
+      </c>
+      <c r="S19" s="16">
+        <v>0.103461</v>
+      </c>
+      <c r="T19" s="16">
+        <v>0.11133800000000001</v>
+      </c>
+      <c r="U19" s="16">
+        <v>0.11884599999999999</v>
+      </c>
+      <c r="V19" s="16">
+        <v>0.12615599999999999</v>
+      </c>
+      <c r="W19" s="16">
+        <v>0.13309799999999999</v>
+      </c>
+      <c r="X19" s="16">
+        <v>0.13953499999999999</v>
+      </c>
+      <c r="Y19" s="16">
+        <v>0.145313</v>
+      </c>
+      <c r="Z19" s="16">
+        <v>0.150369</v>
+      </c>
+      <c r="AA19" s="16">
+        <v>0.15482199999999999</v>
+      </c>
+      <c r="AB19" s="16">
+        <v>0.15862499999999999</v>
+      </c>
+      <c r="AC19" s="16">
+        <v>0.16183400000000001</v>
+      </c>
+      <c r="AD19" s="16">
+        <v>0.164518</v>
+      </c>
+      <c r="AE19" s="16">
+        <v>0.16672400000000001</v>
+      </c>
+      <c r="AF19" s="16">
+        <v>0.168549</v>
+      </c>
+      <c r="AG19" s="16">
+        <v>0.17003399999999999</v>
+      </c>
+      <c r="AH19" s="16">
+        <v>0.17121900000000001</v>
+      </c>
+      <c r="AI19" s="16">
+        <v>0.172178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="14">
+        <f>L7*(1-$B$8)</f>
+        <v>8.7115347055394012E-3</v>
+      </c>
+      <c r="C20" s="14">
+        <f>L8*(1-$B$8)</f>
+        <v>1.7759747080858101E-2</v>
+      </c>
+      <c r="D20" s="14">
+        <f>L9*(1-$B$8)</f>
+        <v>2.1042354361206286E-2</v>
+      </c>
+      <c r="E20" s="14">
+        <f>L10*(1-$B$8)</f>
+        <v>2.1042354361206286E-2</v>
+      </c>
+      <c r="F20" s="14">
+        <f>L11*(1-$B$8)</f>
+        <v>3.5772002414050687E-2</v>
+      </c>
+      <c r="G20" s="14">
+        <f>L12*(1-$B$8)</f>
+        <v>3.808666139378282E-2</v>
+      </c>
+      <c r="H20" s="14">
+        <f>L13*(1-$B$8)</f>
+        <v>4.3827015663519375E-2</v>
+      </c>
+      <c r="I20" s="14">
+        <f>L14*(1-$B$8)</f>
+        <v>4.956736993325743E-2</v>
+      </c>
+      <c r="J20" s="14">
+        <f>L15*(1-$B$8)</f>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="K20" s="14">
+        <f>$J20</f>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="L20" s="14">
+        <f t="shared" ref="L20:AI20" si="3">$J20</f>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="M20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="N20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="O20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="P20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="Q20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="R20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="S20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="T20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="U20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="V20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="W20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="X20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="Y20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="Z20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AA20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AB20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AC20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AD20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AE20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AF20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AG20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AH20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AI20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4">
+        <f>B19+B20</f>
+        <v>5.10119347055394E-2</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" ref="C21:AI21" si="4">C19+C20</f>
+        <v>6.0060147080858106E-2</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="4"/>
+        <v>6.3342754361206288E-2</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="4"/>
+        <v>6.3912154361206286E-2</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="4"/>
+        <v>7.9516502414050685E-2</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="4"/>
+        <v>8.2902161393782814E-2</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="4"/>
+        <v>9.0138715663519373E-2</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="4"/>
+        <v>9.7891869933257436E-2</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.10624972420299397</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.10950872420299398</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.11352602420299399</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.11837592420299398</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.12380752420299398</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.12964302420299398</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.13612592420299399</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.14328402420299396</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.15090832420299397</v>
+      </c>
+      <c r="S21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.15876872420299398</v>
+      </c>
+      <c r="T21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.16664572420299398</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.17415372420299396</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18146372420299398</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18840572420299398</v>
+      </c>
+      <c r="X21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19484272420299398</v>
+      </c>
+      <c r="Y21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20062072420299398</v>
+      </c>
+      <c r="Z21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20567672420299399</v>
+      </c>
+      <c r="AA21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21012972420299397</v>
+      </c>
+      <c r="AB21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21393272420299397</v>
+      </c>
+      <c r="AC21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21714172420299399</v>
+      </c>
+      <c r="AD21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21982572420299398</v>
+      </c>
+      <c r="AE21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.222031724202994</v>
+      </c>
+      <c r="AF21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22385672420299399</v>
+      </c>
+      <c r="AG21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22534172420299398</v>
+      </c>
+      <c r="AH21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.226526724202994</v>
+      </c>
+      <c r="AI21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22748572420299398</v>
       </c>
     </row>
   </sheetData>
@@ -947,7 +1683,7 @@
   <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,144 +1796,144 @@
       </c>
     </row>
     <row r="2" spans="1:35" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3">
-        <f>'India Data'!B2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="C2" s="3">
-        <f>'India Data'!C2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="D2" s="3">
-        <f>'India Data'!D2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="E2" s="3">
-        <f>'India Data'!E2</f>
-        <v>4.6217899999999999E-2</v>
-      </c>
-      <c r="F2" s="3">
-        <f>'India Data'!F2</f>
-        <v>4.7382899999999999E-2</v>
-      </c>
-      <c r="G2" s="3">
-        <f>'India Data'!G2</f>
-        <v>4.8742599999999997E-2</v>
-      </c>
-      <c r="H2" s="3">
-        <f>'India Data'!H2</f>
-        <v>5.0532800000000003E-2</v>
-      </c>
-      <c r="I2" s="3">
-        <f>'India Data'!I2</f>
-        <v>5.2832999999999998E-2</v>
-      </c>
-      <c r="J2" s="3">
-        <f>'India Data'!J2</f>
-        <v>5.5727800000000001E-2</v>
-      </c>
-      <c r="K2" s="3">
-        <f>'India Data'!K2</f>
-        <v>5.9197E-2</v>
-      </c>
-      <c r="L2" s="3">
-        <f>'India Data'!L2</f>
-        <v>6.3418799999999997E-2</v>
-      </c>
-      <c r="M2" s="3">
-        <f>'India Data'!M2</f>
-        <v>6.8455600000000005E-2</v>
-      </c>
-      <c r="N2" s="3">
-        <f>'India Data'!N2</f>
-        <v>7.4057899999999996E-2</v>
-      </c>
-      <c r="O2" s="3">
-        <f>'India Data'!O2</f>
-        <v>8.0028500000000002E-2</v>
-      </c>
-      <c r="P2" s="3">
-        <f>'India Data'!P2</f>
-        <v>8.6307599999999998E-2</v>
-      </c>
-      <c r="Q2" s="3">
-        <f>'India Data'!Q2</f>
-        <v>9.3254299999999998E-2</v>
-      </c>
-      <c r="R2" s="3">
-        <f>'India Data'!R2</f>
-        <v>0.100676</v>
-      </c>
-      <c r="S2" s="3">
-        <f>'India Data'!S2</f>
-        <v>0.10834299999999999</v>
-      </c>
-      <c r="T2" s="3">
-        <f>'India Data'!T2</f>
-        <v>0.116036</v>
-      </c>
-      <c r="U2" s="3">
-        <f>'India Data'!U2</f>
-        <v>0.123373</v>
-      </c>
-      <c r="V2" s="3">
-        <f>'India Data'!V2</f>
-        <v>0.130523</v>
-      </c>
-      <c r="W2" s="3">
-        <f>'India Data'!W2</f>
-        <v>0.137318</v>
-      </c>
-      <c r="X2" s="3">
-        <f>'India Data'!X2</f>
-        <v>0.14362</v>
-      </c>
-      <c r="Y2" s="3">
-        <f>'India Data'!Y2</f>
-        <v>0.14927699999999999</v>
-      </c>
-      <c r="Z2" s="3">
-        <f>'India Data'!Z2</f>
-        <v>0.154227</v>
-      </c>
-      <c r="AA2" s="3">
-        <f>'India Data'!AA2</f>
-        <v>0.15858800000000001</v>
-      </c>
-      <c r="AB2" s="3">
-        <f>'India Data'!AB2</f>
-        <v>0.16231100000000001</v>
-      </c>
-      <c r="AC2" s="3">
-        <f>'India Data'!AC2</f>
-        <v>0.16545099999999999</v>
-      </c>
-      <c r="AD2" s="3">
-        <f>'India Data'!AD2</f>
-        <v>0.168075</v>
-      </c>
-      <c r="AE2" s="3">
-        <f>'India Data'!AE2</f>
-        <v>0.170241</v>
-      </c>
-      <c r="AF2" s="3">
-        <f>'India Data'!AF2</f>
-        <v>0.17203599999999999</v>
-      </c>
-      <c r="AG2" s="3">
-        <f>'India Data'!AG2</f>
-        <v>0.17349800000000001</v>
-      </c>
-      <c r="AH2" s="3">
-        <f>'India Data'!AH2</f>
-        <v>0.17466400000000001</v>
-      </c>
-      <c r="AI2" s="3">
-        <f>'India Data'!AI2</f>
-        <v>0.17560700000000001</v>
+      <c r="A2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="4">
+        <f>'India Data'!B21</f>
+        <v>5.10119347055394E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <f>'India Data'!C21</f>
+        <v>6.0060147080858106E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <f>'India Data'!D21</f>
+        <v>6.3342754361206288E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <f>'India Data'!E21</f>
+        <v>6.3912154361206286E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <f>'India Data'!F21</f>
+        <v>7.9516502414050685E-2</v>
+      </c>
+      <c r="G2" s="4">
+        <f>'India Data'!G21</f>
+        <v>8.2902161393782814E-2</v>
+      </c>
+      <c r="H2" s="4">
+        <f>'India Data'!H21</f>
+        <v>9.0138715663519373E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <f>'India Data'!I21</f>
+        <v>9.7891869933257436E-2</v>
+      </c>
+      <c r="J2" s="4">
+        <f>'India Data'!J21</f>
+        <v>0.10624972420299397</v>
+      </c>
+      <c r="K2" s="4">
+        <f>'India Data'!K21</f>
+        <v>0.10950872420299398</v>
+      </c>
+      <c r="L2" s="4">
+        <f>'India Data'!L21</f>
+        <v>0.11352602420299399</v>
+      </c>
+      <c r="M2" s="4">
+        <f>'India Data'!M21</f>
+        <v>0.11837592420299398</v>
+      </c>
+      <c r="N2" s="4">
+        <f>'India Data'!N21</f>
+        <v>0.12380752420299398</v>
+      </c>
+      <c r="O2" s="4">
+        <f>'India Data'!O21</f>
+        <v>0.12964302420299398</v>
+      </c>
+      <c r="P2" s="4">
+        <f>'India Data'!P21</f>
+        <v>0.13612592420299399</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>'India Data'!Q21</f>
+        <v>0.14328402420299396</v>
+      </c>
+      <c r="R2" s="4">
+        <f>'India Data'!R21</f>
+        <v>0.15090832420299397</v>
+      </c>
+      <c r="S2" s="4">
+        <f>'India Data'!S21</f>
+        <v>0.15876872420299398</v>
+      </c>
+      <c r="T2" s="4">
+        <f>'India Data'!T21</f>
+        <v>0.16664572420299398</v>
+      </c>
+      <c r="U2" s="4">
+        <f>'India Data'!U21</f>
+        <v>0.17415372420299396</v>
+      </c>
+      <c r="V2" s="4">
+        <f>'India Data'!V21</f>
+        <v>0.18146372420299398</v>
+      </c>
+      <c r="W2" s="4">
+        <f>'India Data'!W21</f>
+        <v>0.18840572420299398</v>
+      </c>
+      <c r="X2" s="4">
+        <f>'India Data'!X21</f>
+        <v>0.19484272420299398</v>
+      </c>
+      <c r="Y2" s="4">
+        <f>'India Data'!Y21</f>
+        <v>0.20062072420299398</v>
+      </c>
+      <c r="Z2" s="4">
+        <f>'India Data'!Z21</f>
+        <v>0.20567672420299399</v>
+      </c>
+      <c r="AA2" s="4">
+        <f>'India Data'!AA21</f>
+        <v>0.21012972420299397</v>
+      </c>
+      <c r="AB2" s="4">
+        <f>'India Data'!AB21</f>
+        <v>0.21393272420299397</v>
+      </c>
+      <c r="AC2" s="4">
+        <f>'India Data'!AC21</f>
+        <v>0.21714172420299399</v>
+      </c>
+      <c r="AD2" s="4">
+        <f>'India Data'!AD21</f>
+        <v>0.21982572420299398</v>
+      </c>
+      <c r="AE2" s="4">
+        <f>'India Data'!AE21</f>
+        <v>0.222031724202994</v>
+      </c>
+      <c r="AF2" s="4">
+        <f>'India Data'!AF21</f>
+        <v>0.22385672420299399</v>
+      </c>
+      <c r="AG2" s="4">
+        <f>'India Data'!AG21</f>
+        <v>0.22534172420299398</v>
+      </c>
+      <c r="AH2" s="4">
+        <f>'India Data'!AH21</f>
+        <v>0.226526724202994</v>
+      </c>
+      <c r="AI2" s="4">
+        <f>'India Data'!AI21</f>
+        <v>0.22748572420299398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LCFS and pumped hydro edits from WRI
</commit_message>
<xml_diff>
--- a/InputData/trans/BLP/BAU LCFS Perc.xlsx
+++ b/InputData/trans/BLP/BAU LCFS Perc.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\BLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAFB86EE-DC6A-4922-B6D3-09C903B16909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F58671C7-6C5F-4B29-BB58-3DCED3539B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="India Data" sheetId="6" r:id="rId2"/>
     <sheet name="BLP" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>BLP BAU LCFS Percentage</t>
   </si>
@@ -42,22 +41,85 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>India National Biofuel blending requirement</t>
+  </si>
+  <si>
+    <t>Current Progress on India's Ethanol Blending Program</t>
+  </si>
+  <si>
+    <t>Ministry of Petroleum and Natural Gas/ Press Information Bureau</t>
+  </si>
+  <si>
+    <t>NITI Aayog / Ministry of Petroleum and Natural Gas</t>
+  </si>
+  <si>
+    <t>National Policy on Biofuel</t>
+  </si>
+  <si>
+    <t>Roadmap for Ethanol Blending in India 2020-25</t>
+  </si>
+  <si>
+    <t>https://pib.gov.in/PressReleasePage.aspx?PRID=1575404</t>
+  </si>
+  <si>
+    <t>https://www.niti.gov.in/sites/default/files/2021-06/EthanolBlendingInIndia_compressed.pdf</t>
+  </si>
+  <si>
+    <t>Table 4.2, Pg. 25</t>
+  </si>
+  <si>
+    <t>Advancement of Ethanol blending target</t>
+  </si>
+  <si>
     <t>LCFS Achieved Before Fuel Shifts</t>
   </si>
   <si>
+    <t>Press Information Bureau, Govt. of India</t>
+  </si>
+  <si>
     <t>Data from Vensim variable for BAU scenario</t>
   </si>
   <si>
     <t>Variable name: "Achieved LCFS Percentage before Fuel Shifts"</t>
   </si>
   <si>
+    <t>https://pib.gov.in/PressReleseDetailm.aspx?PRID=1724642</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Trend-based achievement of India's ethanol blending target for petroleum is assumed for the BAU in the BPoEFUbVT variable, </t>
-  </si>
-  <si>
-    <t>The BAU LCFS percentage is set to the BAU Vensim variable "Achieved LCFS Percentage before Fuel Shifts" which accounts for BAU electricity and biofuel blending in transport.</t>
+    <t xml:space="preserve">MoPNG has announced the National Policy on Biofuels in 2018 with a target of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">20% blending of ethanol in petrol and 5% blending of bio-diesel in diesel by 2030. </t>
+  </si>
+  <si>
+    <t>In 2021, the target for petrol was advanced to 2025 from 2030.</t>
+  </si>
+  <si>
+    <t>Due to feedstock supply procurement and land availability constraints, we</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjust this target to a more realistic level by extrapolating </t>
+  </si>
+  <si>
+    <t>the historical trend in target progress between 2014-2021 until 2025.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> We estimate the carbon intensity of the biofuel </t>
+  </si>
+  <si>
+    <t>per litre, relative to conventional petrol (using values from model input file fuels/PEI), to estimate the LCFS percentage.</t>
+  </si>
+  <si>
+    <t>Beyond 2025, we hold the values constant due to lack of credible projections</t>
+  </si>
+  <si>
+    <t>and long-term uncertaintly associated with bio-ethanol feedstock availability.</t>
+  </si>
+  <si>
+    <t>We do not consider the target for diesel as its blending staus as of 2021 is at less than 0.1%</t>
   </si>
   <si>
     <t xml:space="preserve">Since the model includes electricity as a carbon-free source in the LCFS policy, </t>
@@ -66,16 +128,52 @@
     <t xml:space="preserve">the LCFS policy setting should specify an LCFS percentage for biofuels in addition to </t>
   </si>
   <si>
-    <t xml:space="preserve">what is already achieved through BAU electricity-use in the transport sector, and the BAU blending rates already assumed to be achieved in the BPoEFUbVT variable, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">for this policy to take effect for biofuel blending mandates. </t>
-  </si>
-  <si>
-    <t>LCFS achieved before fuel shifts (Vensim)</t>
+    <t xml:space="preserve">what is already achieved through electricity-use in the transport sector for this policy to take effect for biofuel blending mandates. </t>
+  </si>
+  <si>
+    <t>Ethanol supply and Blending status since 2012-'13</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Blending %</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>CO2 emissions intensity (from file fuels/PEI)</t>
+  </si>
+  <si>
+    <t>Petroleum gasoline</t>
+  </si>
+  <si>
+    <t>g/BTU</t>
+  </si>
+  <si>
+    <t>Biofuel gasoline</t>
+  </si>
+  <si>
+    <t>|&lt;-- Historic progress</t>
+  </si>
+  <si>
+    <t>Carbon intensity ratio</t>
+  </si>
+  <si>
+    <t>|&lt;-- Trend based (2017-21) projections</t>
+  </si>
+  <si>
+    <t>LCFS achieved from biofuel gasoline shift</t>
+  </si>
+  <si>
+    <t>India LCFS %</t>
   </si>
   <si>
     <t>BAU LCFS Perc (dimensionless)</t>
+  </si>
+  <si>
+    <t>Achieved LCFS Percentage before Fuel Shifts</t>
   </si>
 </sst>
 </file>
@@ -155,7 +253,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,11 +268,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="53"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -219,6 +323,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="hair">
         <color indexed="64"/>
       </left>
@@ -255,25 +385,49 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="6" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Accent6 2" xfId="11" xr:uid="{083580D2-BB25-4950-82FB-4BC359D4A0E5}"/>
@@ -625,312 +779,894 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="E6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="E7" s="7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>2021</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{FB89C71C-543B-4451-B50F-90BB3D3CC750}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{DB2C66A2-500E-4EC9-85DD-D3844ACC5F91}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{DCCA8351-BB79-43B5-BBBE-AEF82B49DE3B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AI21"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection sqref="A1:XFD17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="B1" s="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K3" s="13">
+        <v>2013</v>
+      </c>
+      <c r="L3" s="17">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="13">
+        <f>K3+1</f>
+        <v>2014</v>
+      </c>
+      <c r="L4" s="17">
+        <v>1.5300000000000001E-2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="14">
+        <v>7.3115370610735544E-2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K5" s="13">
+        <f t="shared" ref="K5:K6" si="0">K4+1</f>
+        <v>2015</v>
+      </c>
+      <c r="L5" s="17">
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="14">
+        <v>4.2344979857895045E-2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K6" s="13">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="L6" s="17">
+        <v>3.5099999999999999E-2</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K7" s="13">
+        <f>K6+1</f>
         <v>2017</v>
       </c>
-      <c r="C1" s="1">
+      <c r="L7" s="17">
+        <v>2.07E-2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8">
+        <f>B6/B5</f>
+        <v>0.57915291277587433</v>
+      </c>
+      <c r="K8" s="13">
+        <f>K7+1</f>
         <v>2018</v>
       </c>
-      <c r="D1" s="1">
+      <c r="L8" s="17">
+        <v>4.2199999999999994E-2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K9" s="13">
+        <f>K8+1</f>
         <v>2019</v>
       </c>
-      <c r="E1" s="1">
+      <c r="L9" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K10" s="13">
+        <f t="shared" ref="K10:K15" si="1">K9+1</f>
         <v>2020</v>
       </c>
-      <c r="F1" s="1">
+      <c r="L10" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="M10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K11" s="13">
+        <f t="shared" si="1"/>
         <v>2021</v>
       </c>
-      <c r="G1" s="1">
+      <c r="L11" s="17">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K12" s="13">
+        <f t="shared" si="1"/>
         <v>2022</v>
       </c>
-      <c r="H1" s="1">
+      <c r="L12" s="18">
+        <f>TREND($L$7:$L$11,$K$7:$K$11,K12)</f>
+        <v>9.0499999999998693E-2</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K13" s="13">
+        <f t="shared" si="1"/>
         <v>2023</v>
       </c>
-      <c r="I1" s="1">
+      <c r="L13" s="18">
+        <f t="shared" ref="L13:L15" si="2">TREND($L$7:$L$11,$K$7:$K$11,K13)</f>
+        <v>0.10413999999999746</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K14" s="13">
+        <f t="shared" si="1"/>
         <v>2024</v>
       </c>
-      <c r="J1" s="1">
+      <c r="L14" s="18">
+        <f t="shared" si="2"/>
+        <v>0.11777999999999977</v>
+      </c>
+      <c r="M14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K15" s="8">
+        <f t="shared" si="1"/>
         <v>2025</v>
       </c>
-      <c r="K1" s="1">
+      <c r="L15" s="18">
+        <f t="shared" si="2"/>
+        <v>0.13141999999999854</v>
+      </c>
+      <c r="M15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2018</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E18" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F18" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2022</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2023</v>
+      </c>
+      <c r="I18" s="1">
+        <v>2024</v>
+      </c>
+      <c r="J18" s="1">
+        <v>2025</v>
+      </c>
+      <c r="K18" s="1">
         <v>2026</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L18" s="1">
         <v>2027</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M18" s="1">
         <v>2028</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N18" s="1">
         <v>2029</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O18" s="1">
         <v>2030</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P18" s="1">
         <v>2031</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q18" s="1">
         <v>2032</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R18" s="1">
         <v>2033</v>
       </c>
-      <c r="S1" s="1">
+      <c r="S18" s="1">
         <v>2034</v>
       </c>
-      <c r="T1" s="1">
+      <c r="T18" s="1">
         <v>2035</v>
       </c>
-      <c r="U1" s="1">
+      <c r="U18" s="1">
         <v>2036</v>
       </c>
-      <c r="V1" s="1">
+      <c r="V18" s="1">
         <v>2037</v>
       </c>
-      <c r="W1" s="1">
+      <c r="W18" s="1">
         <v>2038</v>
       </c>
-      <c r="X1" s="1">
+      <c r="X18" s="1">
         <v>2039</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Y18" s="1">
         <v>2040</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Z18" s="1">
         <v>2041</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AA18" s="1">
         <v>2042</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AB18" s="1">
         <v>2043</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AC18" s="1">
         <v>2044</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AD18" s="1">
         <v>2045</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AE18" s="1">
         <v>2046</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AF18" s="1">
         <v>2047</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="AG18" s="1">
         <v>2048</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="AH18" s="1">
         <v>2049</v>
       </c>
-      <c r="AI1" s="1">
+      <c r="AI18" s="1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3">
-        <f>D2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="C2" s="3">
-        <f>D2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="D2" s="8">
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="E2" s="8">
-        <v>4.6217899999999999E-2</v>
-      </c>
-      <c r="F2" s="8">
-        <v>4.7382899999999999E-2</v>
-      </c>
-      <c r="G2" s="8">
-        <v>4.8742599999999997E-2</v>
-      </c>
-      <c r="H2" s="8">
-        <v>5.0532800000000003E-2</v>
-      </c>
-      <c r="I2" s="8">
-        <v>5.2832999999999998E-2</v>
-      </c>
-      <c r="J2" s="8">
-        <v>5.5727800000000001E-2</v>
-      </c>
-      <c r="K2" s="8">
-        <v>5.9197E-2</v>
-      </c>
-      <c r="L2" s="8">
-        <v>6.3418799999999997E-2</v>
-      </c>
-      <c r="M2" s="8">
-        <v>6.8455600000000005E-2</v>
-      </c>
-      <c r="N2" s="8">
-        <v>7.4057899999999996E-2</v>
-      </c>
-      <c r="O2" s="8">
-        <v>8.0028500000000002E-2</v>
-      </c>
-      <c r="P2" s="8">
-        <v>8.6307599999999998E-2</v>
-      </c>
-      <c r="Q2" s="8">
-        <v>9.3254299999999998E-2</v>
-      </c>
-      <c r="R2" s="8">
-        <v>0.100676</v>
-      </c>
-      <c r="S2" s="8">
-        <v>0.10834299999999999</v>
-      </c>
-      <c r="T2" s="8">
-        <v>0.116036</v>
-      </c>
-      <c r="U2" s="8">
-        <v>0.123373</v>
-      </c>
-      <c r="V2" s="8">
-        <v>0.130523</v>
-      </c>
-      <c r="W2" s="8">
-        <v>0.137318</v>
-      </c>
-      <c r="X2" s="8">
-        <v>0.14362</v>
-      </c>
-      <c r="Y2" s="8">
-        <v>0.14927699999999999</v>
-      </c>
-      <c r="Z2" s="8">
-        <v>0.154227</v>
-      </c>
-      <c r="AA2" s="8">
-        <v>0.15858800000000001</v>
-      </c>
-      <c r="AB2" s="8">
-        <v>0.16231100000000001</v>
-      </c>
-      <c r="AC2" s="8">
-        <v>0.16545099999999999</v>
-      </c>
-      <c r="AD2" s="8">
-        <v>0.168075</v>
-      </c>
-      <c r="AE2" s="8">
-        <v>0.170241</v>
-      </c>
-      <c r="AF2" s="8">
-        <v>0.17203599999999999</v>
-      </c>
-      <c r="AG2" s="8">
-        <v>0.17349800000000001</v>
-      </c>
-      <c r="AH2" s="8">
-        <v>0.17466400000000001</v>
-      </c>
-      <c r="AI2" s="8">
-        <v>0.17560700000000001</v>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="14">
+        <f>D19</f>
+        <v>4.2300400000000002E-2</v>
+      </c>
+      <c r="C19" s="14">
+        <f>D19</f>
+        <v>4.2300400000000002E-2</v>
+      </c>
+      <c r="D19" s="16">
+        <v>4.2300400000000002E-2</v>
+      </c>
+      <c r="E19" s="16">
+        <v>4.28698E-2</v>
+      </c>
+      <c r="F19" s="16">
+        <v>4.3744499999999999E-2</v>
+      </c>
+      <c r="G19" s="16">
+        <v>4.4815500000000001E-2</v>
+      </c>
+      <c r="H19" s="16">
+        <v>4.6311699999999997E-2</v>
+      </c>
+      <c r="I19" s="16">
+        <v>4.8324499999999999E-2</v>
+      </c>
+      <c r="J19" s="16">
+        <v>5.0942000000000001E-2</v>
+      </c>
+      <c r="K19" s="16">
+        <v>5.4200999999999999E-2</v>
+      </c>
+      <c r="L19" s="16">
+        <v>5.8218300000000001E-2</v>
+      </c>
+      <c r="M19" s="16">
+        <v>6.3068200000000005E-2</v>
+      </c>
+      <c r="N19" s="16">
+        <v>6.84998E-2</v>
+      </c>
+      <c r="O19" s="16">
+        <v>7.4335300000000007E-2</v>
+      </c>
+      <c r="P19" s="16">
+        <v>8.0818200000000007E-2</v>
+      </c>
+      <c r="Q19" s="16">
+        <v>8.7976299999999993E-2</v>
+      </c>
+      <c r="R19" s="16">
+        <v>9.5600599999999994E-2</v>
+      </c>
+      <c r="S19" s="16">
+        <v>0.103461</v>
+      </c>
+      <c r="T19" s="16">
+        <v>0.11133800000000001</v>
+      </c>
+      <c r="U19" s="16">
+        <v>0.11884599999999999</v>
+      </c>
+      <c r="V19" s="16">
+        <v>0.12615599999999999</v>
+      </c>
+      <c r="W19" s="16">
+        <v>0.13309799999999999</v>
+      </c>
+      <c r="X19" s="16">
+        <v>0.13953499999999999</v>
+      </c>
+      <c r="Y19" s="16">
+        <v>0.145313</v>
+      </c>
+      <c r="Z19" s="16">
+        <v>0.150369</v>
+      </c>
+      <c r="AA19" s="16">
+        <v>0.15482199999999999</v>
+      </c>
+      <c r="AB19" s="16">
+        <v>0.15862499999999999</v>
+      </c>
+      <c r="AC19" s="16">
+        <v>0.16183400000000001</v>
+      </c>
+      <c r="AD19" s="16">
+        <v>0.164518</v>
+      </c>
+      <c r="AE19" s="16">
+        <v>0.16672400000000001</v>
+      </c>
+      <c r="AF19" s="16">
+        <v>0.168549</v>
+      </c>
+      <c r="AG19" s="16">
+        <v>0.17003399999999999</v>
+      </c>
+      <c r="AH19" s="16">
+        <v>0.17121900000000001</v>
+      </c>
+      <c r="AI19" s="16">
+        <v>0.172178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="14">
+        <f>L7*(1-$B$8)</f>
+        <v>8.7115347055394012E-3</v>
+      </c>
+      <c r="C20" s="14">
+        <f>L8*(1-$B$8)</f>
+        <v>1.7759747080858101E-2</v>
+      </c>
+      <c r="D20" s="14">
+        <f>L9*(1-$B$8)</f>
+        <v>2.1042354361206286E-2</v>
+      </c>
+      <c r="E20" s="14">
+        <f>L10*(1-$B$8)</f>
+        <v>2.1042354361206286E-2</v>
+      </c>
+      <c r="F20" s="14">
+        <f>L11*(1-$B$8)</f>
+        <v>3.5772002414050687E-2</v>
+      </c>
+      <c r="G20" s="14">
+        <f>L12*(1-$B$8)</f>
+        <v>3.808666139378282E-2</v>
+      </c>
+      <c r="H20" s="14">
+        <f>L13*(1-$B$8)</f>
+        <v>4.3827015663519375E-2</v>
+      </c>
+      <c r="I20" s="14">
+        <f>L14*(1-$B$8)</f>
+        <v>4.956736993325743E-2</v>
+      </c>
+      <c r="J20" s="14">
+        <f>L15*(1-$B$8)</f>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="K20" s="14">
+        <f>$J20</f>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="L20" s="14">
+        <f t="shared" ref="L20:AI20" si="3">$J20</f>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="M20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="N20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="O20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="P20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="Q20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="R20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="S20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="T20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="U20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="V20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="W20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="X20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="Y20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="Z20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AA20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AB20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AC20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AD20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AE20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AF20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AG20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AH20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+      <c r="AI20" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5307724202993978E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="4">
+        <f>B19+B20</f>
+        <v>5.10119347055394E-2</v>
+      </c>
+      <c r="C21" s="4">
+        <f t="shared" ref="C21:AI21" si="4">C19+C20</f>
+        <v>6.0060147080858106E-2</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="4"/>
+        <v>6.3342754361206288E-2</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="4"/>
+        <v>6.3912154361206286E-2</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="4"/>
+        <v>7.9516502414050685E-2</v>
+      </c>
+      <c r="G21" s="4">
+        <f t="shared" si="4"/>
+        <v>8.2902161393782814E-2</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="4"/>
+        <v>9.0138715663519373E-2</v>
+      </c>
+      <c r="I21" s="4">
+        <f t="shared" si="4"/>
+        <v>9.7891869933257436E-2</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.10624972420299397</v>
+      </c>
+      <c r="K21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.10950872420299398</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.11352602420299399</v>
+      </c>
+      <c r="M21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.11837592420299398</v>
+      </c>
+      <c r="N21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.12380752420299398</v>
+      </c>
+      <c r="O21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.12964302420299398</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.13612592420299399</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.14328402420299396</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.15090832420299397</v>
+      </c>
+      <c r="S21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.15876872420299398</v>
+      </c>
+      <c r="T21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.16664572420299398</v>
+      </c>
+      <c r="U21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.17415372420299396</v>
+      </c>
+      <c r="V21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18146372420299398</v>
+      </c>
+      <c r="W21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.18840572420299398</v>
+      </c>
+      <c r="X21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.19484272420299398</v>
+      </c>
+      <c r="Y21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20062072420299398</v>
+      </c>
+      <c r="Z21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.20567672420299399</v>
+      </c>
+      <c r="AA21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21012972420299397</v>
+      </c>
+      <c r="AB21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21393272420299397</v>
+      </c>
+      <c r="AC21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21714172420299399</v>
+      </c>
+      <c r="AD21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.21982572420299398</v>
+      </c>
+      <c r="AE21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.222031724202994</v>
+      </c>
+      <c r="AF21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22385672420299399</v>
+      </c>
+      <c r="AG21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22534172420299398</v>
+      </c>
+      <c r="AH21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.226526724202994</v>
+      </c>
+      <c r="AI21" s="4">
+        <f t="shared" si="4"/>
+        <v>0.22748572420299398</v>
       </c>
     </row>
   </sheetData>
@@ -947,7 +1683,7 @@
   <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,144 +1796,144 @@
       </c>
     </row>
     <row r="2" spans="1:35" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3">
-        <f>'India Data'!B2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="C2" s="3">
-        <f>'India Data'!C2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="D2" s="3">
-        <f>'India Data'!D2</f>
-        <v>4.5309799999999997E-2</v>
-      </c>
-      <c r="E2" s="3">
-        <f>'India Data'!E2</f>
-        <v>4.6217899999999999E-2</v>
-      </c>
-      <c r="F2" s="3">
-        <f>'India Data'!F2</f>
-        <v>4.7382899999999999E-2</v>
-      </c>
-      <c r="G2" s="3">
-        <f>'India Data'!G2</f>
-        <v>4.8742599999999997E-2</v>
-      </c>
-      <c r="H2" s="3">
-        <f>'India Data'!H2</f>
-        <v>5.0532800000000003E-2</v>
-      </c>
-      <c r="I2" s="3">
-        <f>'India Data'!I2</f>
-        <v>5.2832999999999998E-2</v>
-      </c>
-      <c r="J2" s="3">
-        <f>'India Data'!J2</f>
-        <v>5.5727800000000001E-2</v>
-      </c>
-      <c r="K2" s="3">
-        <f>'India Data'!K2</f>
-        <v>5.9197E-2</v>
-      </c>
-      <c r="L2" s="3">
-        <f>'India Data'!L2</f>
-        <v>6.3418799999999997E-2</v>
-      </c>
-      <c r="M2" s="3">
-        <f>'India Data'!M2</f>
-        <v>6.8455600000000005E-2</v>
-      </c>
-      <c r="N2" s="3">
-        <f>'India Data'!N2</f>
-        <v>7.4057899999999996E-2</v>
-      </c>
-      <c r="O2" s="3">
-        <f>'India Data'!O2</f>
-        <v>8.0028500000000002E-2</v>
-      </c>
-      <c r="P2" s="3">
-        <f>'India Data'!P2</f>
-        <v>8.6307599999999998E-2</v>
-      </c>
-      <c r="Q2" s="3">
-        <f>'India Data'!Q2</f>
-        <v>9.3254299999999998E-2</v>
-      </c>
-      <c r="R2" s="3">
-        <f>'India Data'!R2</f>
-        <v>0.100676</v>
-      </c>
-      <c r="S2" s="3">
-        <f>'India Data'!S2</f>
-        <v>0.10834299999999999</v>
-      </c>
-      <c r="T2" s="3">
-        <f>'India Data'!T2</f>
-        <v>0.116036</v>
-      </c>
-      <c r="U2" s="3">
-        <f>'India Data'!U2</f>
-        <v>0.123373</v>
-      </c>
-      <c r="V2" s="3">
-        <f>'India Data'!V2</f>
-        <v>0.130523</v>
-      </c>
-      <c r="W2" s="3">
-        <f>'India Data'!W2</f>
-        <v>0.137318</v>
-      </c>
-      <c r="X2" s="3">
-        <f>'India Data'!X2</f>
-        <v>0.14362</v>
-      </c>
-      <c r="Y2" s="3">
-        <f>'India Data'!Y2</f>
-        <v>0.14927699999999999</v>
-      </c>
-      <c r="Z2" s="3">
-        <f>'India Data'!Z2</f>
-        <v>0.154227</v>
-      </c>
-      <c r="AA2" s="3">
-        <f>'India Data'!AA2</f>
-        <v>0.15858800000000001</v>
-      </c>
-      <c r="AB2" s="3">
-        <f>'India Data'!AB2</f>
-        <v>0.16231100000000001</v>
-      </c>
-      <c r="AC2" s="3">
-        <f>'India Data'!AC2</f>
-        <v>0.16545099999999999</v>
-      </c>
-      <c r="AD2" s="3">
-        <f>'India Data'!AD2</f>
-        <v>0.168075</v>
-      </c>
-      <c r="AE2" s="3">
-        <f>'India Data'!AE2</f>
-        <v>0.170241</v>
-      </c>
-      <c r="AF2" s="3">
-        <f>'India Data'!AF2</f>
-        <v>0.17203599999999999</v>
-      </c>
-      <c r="AG2" s="3">
-        <f>'India Data'!AG2</f>
-        <v>0.17349800000000001</v>
-      </c>
-      <c r="AH2" s="3">
-        <f>'India Data'!AH2</f>
-        <v>0.17466400000000001</v>
-      </c>
-      <c r="AI2" s="3">
-        <f>'India Data'!AI2</f>
-        <v>0.17560700000000001</v>
+      <c r="A2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="4">
+        <f>'India Data'!B21</f>
+        <v>5.10119347055394E-2</v>
+      </c>
+      <c r="C2" s="4">
+        <f>'India Data'!C21</f>
+        <v>6.0060147080858106E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <f>'India Data'!D21</f>
+        <v>6.3342754361206288E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <f>'India Data'!E21</f>
+        <v>6.3912154361206286E-2</v>
+      </c>
+      <c r="F2" s="4">
+        <f>'India Data'!F21</f>
+        <v>7.9516502414050685E-2</v>
+      </c>
+      <c r="G2" s="4">
+        <f>'India Data'!G21</f>
+        <v>8.2902161393782814E-2</v>
+      </c>
+      <c r="H2" s="4">
+        <f>'India Data'!H21</f>
+        <v>9.0138715663519373E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <f>'India Data'!I21</f>
+        <v>9.7891869933257436E-2</v>
+      </c>
+      <c r="J2" s="4">
+        <f>'India Data'!J21</f>
+        <v>0.10624972420299397</v>
+      </c>
+      <c r="K2" s="4">
+        <f>'India Data'!K21</f>
+        <v>0.10950872420299398</v>
+      </c>
+      <c r="L2" s="4">
+        <f>'India Data'!L21</f>
+        <v>0.11352602420299399</v>
+      </c>
+      <c r="M2" s="4">
+        <f>'India Data'!M21</f>
+        <v>0.11837592420299398</v>
+      </c>
+      <c r="N2" s="4">
+        <f>'India Data'!N21</f>
+        <v>0.12380752420299398</v>
+      </c>
+      <c r="O2" s="4">
+        <f>'India Data'!O21</f>
+        <v>0.12964302420299398</v>
+      </c>
+      <c r="P2" s="4">
+        <f>'India Data'!P21</f>
+        <v>0.13612592420299399</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>'India Data'!Q21</f>
+        <v>0.14328402420299396</v>
+      </c>
+      <c r="R2" s="4">
+        <f>'India Data'!R21</f>
+        <v>0.15090832420299397</v>
+      </c>
+      <c r="S2" s="4">
+        <f>'India Data'!S21</f>
+        <v>0.15876872420299398</v>
+      </c>
+      <c r="T2" s="4">
+        <f>'India Data'!T21</f>
+        <v>0.16664572420299398</v>
+      </c>
+      <c r="U2" s="4">
+        <f>'India Data'!U21</f>
+        <v>0.17415372420299396</v>
+      </c>
+      <c r="V2" s="4">
+        <f>'India Data'!V21</f>
+        <v>0.18146372420299398</v>
+      </c>
+      <c r="W2" s="4">
+        <f>'India Data'!W21</f>
+        <v>0.18840572420299398</v>
+      </c>
+      <c r="X2" s="4">
+        <f>'India Data'!X21</f>
+        <v>0.19484272420299398</v>
+      </c>
+      <c r="Y2" s="4">
+        <f>'India Data'!Y21</f>
+        <v>0.20062072420299398</v>
+      </c>
+      <c r="Z2" s="4">
+        <f>'India Data'!Z21</f>
+        <v>0.20567672420299399</v>
+      </c>
+      <c r="AA2" s="4">
+        <f>'India Data'!AA21</f>
+        <v>0.21012972420299397</v>
+      </c>
+      <c r="AB2" s="4">
+        <f>'India Data'!AB21</f>
+        <v>0.21393272420299397</v>
+      </c>
+      <c r="AC2" s="4">
+        <f>'India Data'!AC21</f>
+        <v>0.21714172420299399</v>
+      </c>
+      <c r="AD2" s="4">
+        <f>'India Data'!AD21</f>
+        <v>0.21982572420299398</v>
+      </c>
+      <c r="AE2" s="4">
+        <f>'India Data'!AE21</f>
+        <v>0.222031724202994</v>
+      </c>
+      <c r="AF2" s="4">
+        <f>'India Data'!AF21</f>
+        <v>0.22385672420299399</v>
+      </c>
+      <c r="AG2" s="4">
+        <f>'India Data'!AG21</f>
+        <v>0.22534172420299398</v>
+      </c>
+      <c r="AH2" s="4">
+        <f>'India Data'!AH21</f>
+        <v>0.226526724202994</v>
+      </c>
+      <c r="AI2" s="4">
+        <f>'India Data'!AI21</f>
+        <v>0.22748572420299398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WRI edits for files that use Vensim outputs
</commit_message>
<xml_diff>
--- a/InputData/trans/BLP/BAU LCFS Perc.xlsx
+++ b/InputData/trans/BLP/BAU LCFS Perc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-india\InputData\trans\BLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F58671C7-6C5F-4B29-BB58-3DCED3539B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7173092-5FB4-4FD2-B0A2-7C1FEDF6715D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -390,7 +390,7 @@
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -425,7 +425,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="6" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -785,18 +784,18 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" customWidth="1"/>
+    <col min="2" max="2" width="56.7265625" customWidth="1"/>
+    <col min="5" max="5" width="53.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -807,7 +806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -815,7 +814,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>2019</v>
       </c>
@@ -823,7 +822,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -831,7 +830,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
@@ -839,13 +838,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B8" s="7"/>
       <c r="E8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
@@ -853,7 +852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>13</v>
       </c>
@@ -861,7 +860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B12" s="10">
         <v>2021</v>
       </c>
@@ -869,82 +868,82 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B13" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -965,21 +964,21 @@
   <dimension ref="A1:AI21"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A24" sqref="A24:AG30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" customWidth="1"/>
+    <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K2" s="11" t="s">
         <v>33</v>
       </c>
@@ -987,18 +986,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K3" s="13">
         <v>2013</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="16">
         <v>6.7000000000000002E-3</v>
       </c>
       <c r="M3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1006,14 +1005,14 @@
         <f>K3+1</f>
         <v>2014</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="16">
         <v>1.5300000000000001E-2</v>
       </c>
       <c r="M4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1027,14 +1026,14 @@
         <f t="shared" ref="K5:K6" si="0">K4+1</f>
         <v>2015</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="16">
         <v>2.3300000000000001E-2</v>
       </c>
       <c r="M5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1048,26 +1047,26 @@
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="16">
         <v>3.5099999999999999E-2</v>
       </c>
       <c r="M6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K7" s="13">
         <f>K6+1</f>
         <v>2017</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7" s="16">
         <v>2.07E-2</v>
       </c>
       <c r="M7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -1079,55 +1078,55 @@
         <f>K7+1</f>
         <v>2018</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>4.2199999999999994E-2</v>
       </c>
       <c r="M8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K9" s="13">
         <f>K8+1</f>
         <v>2019</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9" s="16">
         <v>0.05</v>
       </c>
       <c r="M9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K10" s="13">
         <f t="shared" ref="K10:K15" si="1">K9+1</f>
         <v>2020</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="16">
         <v>0.05</v>
       </c>
       <c r="M10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K11" s="13">
         <f t="shared" si="1"/>
         <v>2021</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="16">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="M11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K12" s="13">
         <f t="shared" si="1"/>
         <v>2022</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="17">
         <f>TREND($L$7:$L$11,$K$7:$K$11,K12)</f>
         <v>9.0499999999998693E-2</v>
       </c>
@@ -1135,12 +1134,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K13" s="13">
         <f t="shared" si="1"/>
         <v>2023</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="17">
         <f t="shared" ref="L13:L15" si="2">TREND($L$7:$L$11,$K$7:$K$11,K13)</f>
         <v>0.10413999999999746</v>
       </c>
@@ -1148,12 +1147,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K14" s="13">
         <f t="shared" si="1"/>
         <v>2024</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="17">
         <f t="shared" si="2"/>
         <v>0.11777999999999977</v>
       </c>
@@ -1161,12 +1160,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K15" s="8">
         <f t="shared" si="1"/>
         <v>2025</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="17">
         <f t="shared" si="2"/>
         <v>0.13141999999999854</v>
       </c>
@@ -1174,7 +1173,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
         <v>2017</v>
       </c>
@@ -1278,116 +1277,116 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="14">
         <f>D19</f>
-        <v>4.2300400000000002E-2</v>
+        <v>8.7927999999999999E-3</v>
       </c>
       <c r="C19" s="14">
         <f>D19</f>
-        <v>4.2300400000000002E-2</v>
-      </c>
-      <c r="D19" s="16">
-        <v>4.2300400000000002E-2</v>
-      </c>
-      <c r="E19" s="16">
-        <v>4.28698E-2</v>
-      </c>
-      <c r="F19" s="16">
-        <v>4.3744499999999999E-2</v>
-      </c>
-      <c r="G19" s="16">
-        <v>4.4815500000000001E-2</v>
-      </c>
-      <c r="H19" s="16">
-        <v>4.6311699999999997E-2</v>
-      </c>
-      <c r="I19" s="16">
-        <v>4.8324499999999999E-2</v>
-      </c>
-      <c r="J19" s="16">
-        <v>5.0942000000000001E-2</v>
-      </c>
-      <c r="K19" s="16">
-        <v>5.4200999999999999E-2</v>
-      </c>
-      <c r="L19" s="16">
-        <v>5.8218300000000001E-2</v>
-      </c>
-      <c r="M19" s="16">
-        <v>6.3068200000000005E-2</v>
-      </c>
-      <c r="N19" s="16">
-        <v>6.84998E-2</v>
-      </c>
-      <c r="O19" s="16">
-        <v>7.4335300000000007E-2</v>
-      </c>
-      <c r="P19" s="16">
-        <v>8.0818200000000007E-2</v>
-      </c>
-      <c r="Q19" s="16">
-        <v>8.7976299999999993E-2</v>
-      </c>
-      <c r="R19" s="16">
-        <v>9.5600599999999994E-2</v>
-      </c>
-      <c r="S19" s="16">
-        <v>0.103461</v>
-      </c>
-      <c r="T19" s="16">
-        <v>0.11133800000000001</v>
-      </c>
-      <c r="U19" s="16">
-        <v>0.11884599999999999</v>
-      </c>
-      <c r="V19" s="16">
-        <v>0.12615599999999999</v>
-      </c>
-      <c r="W19" s="16">
-        <v>0.13309799999999999</v>
-      </c>
-      <c r="X19" s="16">
-        <v>0.13953499999999999</v>
-      </c>
-      <c r="Y19" s="16">
-        <v>0.145313</v>
-      </c>
-      <c r="Z19" s="16">
-        <v>0.150369</v>
-      </c>
-      <c r="AA19" s="16">
-        <v>0.15482199999999999</v>
-      </c>
-      <c r="AB19" s="16">
-        <v>0.15862499999999999</v>
-      </c>
-      <c r="AC19" s="16">
-        <v>0.16183400000000001</v>
-      </c>
-      <c r="AD19" s="16">
-        <v>0.164518</v>
-      </c>
-      <c r="AE19" s="16">
-        <v>0.16672400000000001</v>
-      </c>
-      <c r="AF19" s="16">
-        <v>0.168549</v>
-      </c>
-      <c r="AG19" s="16">
-        <v>0.17003399999999999</v>
-      </c>
-      <c r="AH19" s="16">
-        <v>0.17121900000000001</v>
-      </c>
-      <c r="AI19" s="16">
-        <v>0.172178</v>
-      </c>
-    </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+        <v>8.7927999999999999E-3</v>
+      </c>
+      <c r="D19">
+        <v>8.7927999999999999E-3</v>
+      </c>
+      <c r="E19">
+        <v>9.6548399999999996E-3</v>
+      </c>
+      <c r="F19">
+        <v>1.1037699999999999E-2</v>
+      </c>
+      <c r="G19">
+        <v>1.30384E-2</v>
+      </c>
+      <c r="H19">
+        <v>1.5729699999999999E-2</v>
+      </c>
+      <c r="I19">
+        <v>1.92914E-2</v>
+      </c>
+      <c r="J19">
+        <v>2.3074399999999998E-2</v>
+      </c>
+      <c r="K19">
+        <v>2.7817000000000001E-2</v>
+      </c>
+      <c r="L19">
+        <v>3.35646E-2</v>
+      </c>
+      <c r="M19">
+        <v>3.9949800000000001E-2</v>
+      </c>
+      <c r="N19">
+        <v>4.6915900000000003E-2</v>
+      </c>
+      <c r="O19">
+        <v>5.45567E-2</v>
+      </c>
+      <c r="P19">
+        <v>6.31771E-2</v>
+      </c>
+      <c r="Q19">
+        <v>7.2533299999999995E-2</v>
+      </c>
+      <c r="R19">
+        <v>8.2414799999999996E-2</v>
+      </c>
+      <c r="S19">
+        <v>9.2526499999999998E-2</v>
+      </c>
+      <c r="T19">
+        <v>0.10312</v>
+      </c>
+      <c r="U19">
+        <v>0.11357</v>
+      </c>
+      <c r="V19">
+        <v>0.123498</v>
+      </c>
+      <c r="W19">
+        <v>0.13272900000000001</v>
+      </c>
+      <c r="X19">
+        <v>0.14150499999999999</v>
+      </c>
+      <c r="Y19">
+        <v>0.14960799999999999</v>
+      </c>
+      <c r="Z19">
+        <v>0.157028</v>
+      </c>
+      <c r="AA19">
+        <v>0.163794</v>
+      </c>
+      <c r="AB19">
+        <v>0.16993800000000001</v>
+      </c>
+      <c r="AC19">
+        <v>0.17538999999999999</v>
+      </c>
+      <c r="AD19">
+        <v>0.18020900000000001</v>
+      </c>
+      <c r="AE19">
+        <v>0.184387</v>
+      </c>
+      <c r="AF19">
+        <v>0.18806300000000001</v>
+      </c>
+      <c r="AG19">
+        <v>0.19123200000000001</v>
+      </c>
+      <c r="AH19">
+        <v>0.19394700000000001</v>
+      </c>
+      <c r="AI19">
+        <v>0.19626399999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1528,145 +1527,145 @@
         <v>5.5307724202993978E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="4">
         <f>B19+B20</f>
-        <v>5.10119347055394E-2</v>
+        <v>1.7504334705539401E-2</v>
       </c>
       <c r="C21" s="4">
         <f t="shared" ref="C21:AI21" si="4">C19+C20</f>
-        <v>6.0060147080858106E-2</v>
+        <v>2.6552547080858101E-2</v>
       </c>
       <c r="D21" s="4">
         <f t="shared" si="4"/>
-        <v>6.3342754361206288E-2</v>
+        <v>2.9835154361206286E-2</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="4"/>
-        <v>6.3912154361206286E-2</v>
+        <v>3.0697194361206284E-2</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="4"/>
-        <v>7.9516502414050685E-2</v>
+        <v>4.6809702414050684E-2</v>
       </c>
       <c r="G21" s="4">
         <f t="shared" si="4"/>
-        <v>8.2902161393782814E-2</v>
+        <v>5.1125061393782818E-2</v>
       </c>
       <c r="H21" s="4">
         <f t="shared" si="4"/>
-        <v>9.0138715663519373E-2</v>
+        <v>5.9556715663519375E-2</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" si="4"/>
-        <v>9.7891869933257436E-2</v>
+        <v>6.885876993325743E-2</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="4"/>
-        <v>0.10624972420299397</v>
+        <v>7.838212420299398E-2</v>
       </c>
       <c r="K21" s="4">
         <f t="shared" si="4"/>
-        <v>0.10950872420299398</v>
+        <v>8.312472420299398E-2</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="4"/>
-        <v>0.11352602420299399</v>
+        <v>8.8872324202993985E-2</v>
       </c>
       <c r="M21" s="4">
         <f t="shared" si="4"/>
-        <v>0.11837592420299398</v>
+        <v>9.5257524202993979E-2</v>
       </c>
       <c r="N21" s="4">
         <f t="shared" si="4"/>
-        <v>0.12380752420299398</v>
+        <v>0.10222362420299398</v>
       </c>
       <c r="O21" s="4">
         <f t="shared" si="4"/>
-        <v>0.12964302420299398</v>
+        <v>0.10986442420299397</v>
       </c>
       <c r="P21" s="4">
         <f t="shared" si="4"/>
-        <v>0.13612592420299399</v>
+        <v>0.11848482420299397</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="4"/>
-        <v>0.14328402420299396</v>
+        <v>0.12784102420299398</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="4"/>
-        <v>0.15090832420299397</v>
+        <v>0.13772252420299397</v>
       </c>
       <c r="S21" s="4">
         <f t="shared" si="4"/>
-        <v>0.15876872420299398</v>
+        <v>0.14783422420299397</v>
       </c>
       <c r="T21" s="4">
         <f t="shared" si="4"/>
-        <v>0.16664572420299398</v>
+        <v>0.15842772420299397</v>
       </c>
       <c r="U21" s="4">
         <f t="shared" si="4"/>
-        <v>0.17415372420299396</v>
+        <v>0.16887772420299399</v>
       </c>
       <c r="V21" s="4">
         <f t="shared" si="4"/>
-        <v>0.18146372420299398</v>
+        <v>0.17880572420299398</v>
       </c>
       <c r="W21" s="4">
         <f t="shared" si="4"/>
-        <v>0.18840572420299398</v>
+        <v>0.188036724202994</v>
       </c>
       <c r="X21" s="4">
         <f t="shared" si="4"/>
-        <v>0.19484272420299398</v>
+        <v>0.19681272420299398</v>
       </c>
       <c r="Y21" s="4">
         <f t="shared" si="4"/>
-        <v>0.20062072420299398</v>
+        <v>0.20491572420299398</v>
       </c>
       <c r="Z21" s="4">
         <f t="shared" si="4"/>
-        <v>0.20567672420299399</v>
+        <v>0.21233572420299399</v>
       </c>
       <c r="AA21" s="4">
         <f t="shared" si="4"/>
-        <v>0.21012972420299397</v>
+        <v>0.21910172420299398</v>
       </c>
       <c r="AB21" s="4">
         <f t="shared" si="4"/>
-        <v>0.21393272420299397</v>
+        <v>0.22524572420299399</v>
       </c>
       <c r="AC21" s="4">
         <f t="shared" si="4"/>
-        <v>0.21714172420299399</v>
+        <v>0.23069772420299398</v>
       </c>
       <c r="AD21" s="4">
         <f t="shared" si="4"/>
-        <v>0.21982572420299398</v>
+        <v>0.23551672420299399</v>
       </c>
       <c r="AE21" s="4">
         <f t="shared" si="4"/>
-        <v>0.222031724202994</v>
+        <v>0.23969472420299398</v>
       </c>
       <c r="AF21" s="4">
         <f t="shared" si="4"/>
-        <v>0.22385672420299399</v>
+        <v>0.24337072420299399</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" si="4"/>
-        <v>0.22534172420299398</v>
+        <v>0.246539724202994</v>
       </c>
       <c r="AH21" s="4">
         <f t="shared" si="4"/>
-        <v>0.226526724202994</v>
+        <v>0.24925472420299399</v>
       </c>
       <c r="AI21" s="4">
         <f t="shared" si="4"/>
-        <v>0.22748572420299398</v>
+        <v>0.25157172420299395</v>
       </c>
     </row>
   </sheetData>
@@ -1686,12 +1685,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>2017</v>
       </c>
@@ -1795,145 +1794,145 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="4">
         <f>'India Data'!B21</f>
-        <v>5.10119347055394E-2</v>
+        <v>1.7504334705539401E-2</v>
       </c>
       <c r="C2" s="4">
         <f>'India Data'!C21</f>
-        <v>6.0060147080858106E-2</v>
+        <v>2.6552547080858101E-2</v>
       </c>
       <c r="D2" s="4">
         <f>'India Data'!D21</f>
-        <v>6.3342754361206288E-2</v>
+        <v>2.9835154361206286E-2</v>
       </c>
       <c r="E2" s="4">
         <f>'India Data'!E21</f>
-        <v>6.3912154361206286E-2</v>
+        <v>3.0697194361206284E-2</v>
       </c>
       <c r="F2" s="4">
         <f>'India Data'!F21</f>
-        <v>7.9516502414050685E-2</v>
+        <v>4.6809702414050684E-2</v>
       </c>
       <c r="G2" s="4">
         <f>'India Data'!G21</f>
-        <v>8.2902161393782814E-2</v>
+        <v>5.1125061393782818E-2</v>
       </c>
       <c r="H2" s="4">
         <f>'India Data'!H21</f>
-        <v>9.0138715663519373E-2</v>
+        <v>5.9556715663519375E-2</v>
       </c>
       <c r="I2" s="4">
         <f>'India Data'!I21</f>
-        <v>9.7891869933257436E-2</v>
+        <v>6.885876993325743E-2</v>
       </c>
       <c r="J2" s="4">
         <f>'India Data'!J21</f>
-        <v>0.10624972420299397</v>
+        <v>7.838212420299398E-2</v>
       </c>
       <c r="K2" s="4">
         <f>'India Data'!K21</f>
-        <v>0.10950872420299398</v>
+        <v>8.312472420299398E-2</v>
       </c>
       <c r="L2" s="4">
         <f>'India Data'!L21</f>
-        <v>0.11352602420299399</v>
+        <v>8.8872324202993985E-2</v>
       </c>
       <c r="M2" s="4">
         <f>'India Data'!M21</f>
-        <v>0.11837592420299398</v>
+        <v>9.5257524202993979E-2</v>
       </c>
       <c r="N2" s="4">
         <f>'India Data'!N21</f>
-        <v>0.12380752420299398</v>
+        <v>0.10222362420299398</v>
       </c>
       <c r="O2" s="4">
         <f>'India Data'!O21</f>
-        <v>0.12964302420299398</v>
+        <v>0.10986442420299397</v>
       </c>
       <c r="P2" s="4">
         <f>'India Data'!P21</f>
-        <v>0.13612592420299399</v>
+        <v>0.11848482420299397</v>
       </c>
       <c r="Q2" s="4">
         <f>'India Data'!Q21</f>
-        <v>0.14328402420299396</v>
+        <v>0.12784102420299398</v>
       </c>
       <c r="R2" s="4">
         <f>'India Data'!R21</f>
-        <v>0.15090832420299397</v>
+        <v>0.13772252420299397</v>
       </c>
       <c r="S2" s="4">
         <f>'India Data'!S21</f>
-        <v>0.15876872420299398</v>
+        <v>0.14783422420299397</v>
       </c>
       <c r="T2" s="4">
         <f>'India Data'!T21</f>
-        <v>0.16664572420299398</v>
+        <v>0.15842772420299397</v>
       </c>
       <c r="U2" s="4">
         <f>'India Data'!U21</f>
-        <v>0.17415372420299396</v>
+        <v>0.16887772420299399</v>
       </c>
       <c r="V2" s="4">
         <f>'India Data'!V21</f>
-        <v>0.18146372420299398</v>
+        <v>0.17880572420299398</v>
       </c>
       <c r="W2" s="4">
         <f>'India Data'!W21</f>
-        <v>0.18840572420299398</v>
+        <v>0.188036724202994</v>
       </c>
       <c r="X2" s="4">
         <f>'India Data'!X21</f>
-        <v>0.19484272420299398</v>
+        <v>0.19681272420299398</v>
       </c>
       <c r="Y2" s="4">
         <f>'India Data'!Y21</f>
-        <v>0.20062072420299398</v>
+        <v>0.20491572420299398</v>
       </c>
       <c r="Z2" s="4">
         <f>'India Data'!Z21</f>
-        <v>0.20567672420299399</v>
+        <v>0.21233572420299399</v>
       </c>
       <c r="AA2" s="4">
         <f>'India Data'!AA21</f>
-        <v>0.21012972420299397</v>
+        <v>0.21910172420299398</v>
       </c>
       <c r="AB2" s="4">
         <f>'India Data'!AB21</f>
-        <v>0.21393272420299397</v>
+        <v>0.22524572420299399</v>
       </c>
       <c r="AC2" s="4">
         <f>'India Data'!AC21</f>
-        <v>0.21714172420299399</v>
+        <v>0.23069772420299398</v>
       </c>
       <c r="AD2" s="4">
         <f>'India Data'!AD21</f>
-        <v>0.21982572420299398</v>
+        <v>0.23551672420299399</v>
       </c>
       <c r="AE2" s="4">
         <f>'India Data'!AE21</f>
-        <v>0.222031724202994</v>
+        <v>0.23969472420299398</v>
       </c>
       <c r="AF2" s="4">
         <f>'India Data'!AF21</f>
-        <v>0.22385672420299399</v>
+        <v>0.24337072420299399</v>
       </c>
       <c r="AG2" s="4">
         <f>'India Data'!AG21</f>
-        <v>0.22534172420299398</v>
+        <v>0.246539724202994</v>
       </c>
       <c r="AH2" s="4">
         <f>'India Data'!AH21</f>
-        <v>0.226526724202994</v>
+        <v>0.24925472420299399</v>
       </c>
       <c r="AI2" s="4">
         <f>'India Data'!AI21</f>
-        <v>0.22748572420299398</v>
+        <v>0.25157172420299395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>